<commit_message>
Changed evaluation of connected clients logic
</commit_message>
<xml_diff>
--- a/docs/Pasta1.xlsx
+++ b/docs/Pasta1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="33">
   <si>
     <t>x</t>
   </si>
@@ -24,46 +24,13 @@
     <t>G(x)</t>
   </si>
   <si>
-    <t>0.1254    0.1987    0.1403   -0.0692   -0.1606   -0.2346</t>
-  </si>
-  <si>
     <t>w1</t>
-  </si>
-  <si>
-    <t>p1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -0.2384    0.0803    0.1219    0.0298    0.0047    0.0016</t>
-  </si>
-  <si>
-    <t>x1</t>
-  </si>
-  <si>
-    <t>x2</t>
-  </si>
-  <si>
-    <t>x3</t>
-  </si>
-  <si>
-    <t>x4</t>
-  </si>
-  <si>
-    <t>x5</t>
-  </si>
-  <si>
-    <t>x6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.3267    0.2915    0.1731   -0.1288   -0.2690   -0.3933</t>
   </si>
   <si>
     <t>w2</t>
   </si>
   <si>
     <t>w3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.3451    0.2855    0.1703   -0.1452   -0.2809   -0.3749</t>
   </si>
   <si>
     <r>
@@ -114,102 +81,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6</t>
-    </r>
-  </si>
-  <si>
     <t>Distância</t>
   </si>
   <si>
@@ -228,29 +99,84 @@
     <t>f2</t>
   </si>
   <si>
-    <t>14.0000   38.9449</t>
+    <t>s1</t>
   </si>
   <si>
-    <t xml:space="preserve">   15.0000   37.3519</t>
+    <t>s2</t>
   </si>
   <si>
-    <t xml:space="preserve">   16.0000   36.8864</t>
+    <t>s3</t>
   </si>
   <si>
-    <t xml:space="preserve">   18.0000   36.5970</t>
+    <t>s4</t>
   </si>
   <si>
-    <t xml:space="preserve">   19.0000   36.3928</t>
+    <t>s5</t>
   </si>
   <si>
-    <t xml:space="preserve">   20.0000   36.1534</t>
+    <t>s6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0     0     0     0</t>
+  </si>
+  <si>
+    <t>6.0000    2.9385    7.2411 0</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <r>
+      <t>w</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>Disconnected Clients</t>
+  </si>
+  <si>
+    <t>Unused Band</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>w4</t>
+  </si>
+  <si>
+    <t>0.1667</t>
+  </si>
+  <si>
+    <t>TotalAP</t>
+  </si>
+  <si>
+    <t>Negative Flux</t>
+  </si>
+  <si>
+    <t>Posive Flux</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,8 +200,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,8 +238,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -330,11 +268,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -366,6 +334,33 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,11 +444,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="96705920"/>
-        <c:axId val="96704384"/>
+        <c:axId val="85147008"/>
+        <c:axId val="86385792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96705920"/>
+        <c:axId val="85147008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -462,13 +457,13 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96704384"/>
+        <c:crossAx val="86385792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.25"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96704384"/>
+        <c:axId val="86385792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -477,7 +472,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96705920"/>
+        <c:crossAx val="85147008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -487,7 +482,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -510,7 +505,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x1</c:v>
+                  <c:v>s1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -554,7 +549,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x2</c:v>
+                  <c:v>s2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -598,7 +593,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x3</c:v>
+                  <c:v>s3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -642,7 +637,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x4</c:v>
+                  <c:v>s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -686,7 +681,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x5</c:v>
+                  <c:v>s5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -730,7 +725,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x6</c:v>
+                  <c:v>s6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -765,11 +760,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="97327744"/>
-        <c:axId val="97325056"/>
+        <c:axId val="87102208"/>
+        <c:axId val="87103744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97327744"/>
+        <c:axId val="87102208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -778,12 +773,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97325056"/>
+        <c:crossAx val="87103744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97325056"/>
+        <c:axId val="87103744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -791,7 +786,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97327744"/>
+        <c:crossAx val="87102208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -804,7 +799,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -827,7 +822,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x1</c:v>
+                  <c:v>s1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -871,7 +866,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x2</c:v>
+                  <c:v>s2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -915,7 +910,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x3</c:v>
+                  <c:v>s3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -959,7 +954,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x4</c:v>
+                  <c:v>s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1003,7 +998,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x5</c:v>
+                  <c:v>s5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1047,7 +1042,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x6</c:v>
+                  <c:v>s6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1082,11 +1077,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="92026368"/>
-        <c:axId val="92039040"/>
+        <c:axId val="87152128"/>
+        <c:axId val="87153664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92026368"/>
+        <c:axId val="87152128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1095,12 +1090,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92039040"/>
+        <c:crossAx val="87153664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92039040"/>
+        <c:axId val="87153664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1108,7 +1103,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92026368"/>
+        <c:crossAx val="87152128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1121,7 +1116,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000041" footer="0.31496062000000041"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1144,7 +1139,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x1</c:v>
+                  <c:v>s1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1188,7 +1183,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x2</c:v>
+                  <c:v>s2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1232,7 +1227,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x3</c:v>
+                  <c:v>s3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1276,7 +1271,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x4</c:v>
+                  <c:v>s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1320,7 +1315,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x5</c:v>
+                  <c:v>s5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1364,7 +1359,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x6</c:v>
+                  <c:v>s6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1399,11 +1394,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="110865792"/>
-        <c:axId val="110885504"/>
+        <c:axId val="87202048"/>
+        <c:axId val="87207936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110865792"/>
+        <c:axId val="87202048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1412,12 +1407,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110885504"/>
+        <c:crossAx val="87207936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110885504"/>
+        <c:axId val="87207936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1420,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110865792"/>
+        <c:crossAx val="87202048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1438,7 +1433,641 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000047" footer="0.31496062000000047"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.25009999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.24510000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.15409999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-0.1099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-0.22550000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-0.31390000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="115270016"/>
+        <c:axId val="115271552"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="115270016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.2"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="115271552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="115271552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="115270016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.18809999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.23169999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.1527</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-8.5800000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-0.1948</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$G$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>s6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$E$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$F$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-0.29189999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="87220224"/>
+        <c:axId val="87223680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="87220224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.2"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87223680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="87223680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87220224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1561,6 +2190,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>31936</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>42582</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>31936</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>64994</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1854,10 +2543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:O64"/>
+  <dimension ref="B1:O93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50:O56"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41:O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1910,30 +2599,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
-      <c r="B22" t="s">
+    <row r="27" spans="4:7">
+      <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="D27" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="F27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7">
       <c r="D28" s="1">
         <v>0.2</v>
       </c>
@@ -1944,10 +2618,10 @@
         <v>-0.2384</v>
       </c>
       <c r="G28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7">
       <c r="D29" s="1">
         <v>0.6</v>
       </c>
@@ -1958,10 +2632,10 @@
         <v>8.0299999999999996E-2</v>
       </c>
       <c r="G29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7">
       <c r="D30" s="1">
         <v>0.2</v>
       </c>
@@ -1972,10 +2646,10 @@
         <v>0.12189999999999999</v>
       </c>
       <c r="G30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7">
       <c r="D31" s="1">
         <v>0</v>
       </c>
@@ -1986,10 +2660,10 @@
         <v>2.98E-2</v>
       </c>
       <c r="G31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7">
       <c r="E32">
         <v>1</v>
       </c>
@@ -1997,10 +2671,10 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="G32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="4:15">
       <c r="E33">
         <v>1</v>
       </c>
@@ -2008,15 +2682,18 @@
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="4:15">
       <c r="D35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="4:15">
       <c r="D36">
         <v>0.6</v>
       </c>
@@ -2027,7 +2704,7 @@
         <v>0.32669999999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:15">
+    <row r="37" spans="4:15">
       <c r="D37">
         <v>0.2</v>
       </c>
@@ -2038,7 +2715,7 @@
         <v>0.29149999999999998</v>
       </c>
     </row>
-    <row r="38" spans="2:15">
+    <row r="38" spans="4:15">
       <c r="D38">
         <v>0.2</v>
       </c>
@@ -2049,7 +2726,7 @@
         <v>0.1731</v>
       </c>
     </row>
-    <row r="39" spans="2:15">
+    <row r="39" spans="4:15">
       <c r="D39">
         <v>0</v>
       </c>
@@ -2060,7 +2737,7 @@
         <v>-0.1288</v>
       </c>
     </row>
-    <row r="40" spans="2:15">
+    <row r="40" spans="4:15">
       <c r="E40">
         <v>1</v>
       </c>
@@ -2069,16 +2746,16 @@
       </c>
       <c r="L40" s="2"/>
       <c r="M40" s="3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="2:15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="4:15">
       <c r="E41">
         <v>1</v>
       </c>
@@ -2086,7 +2763,7 @@
         <v>-0.39329999999999998</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="M41" s="8">
         <v>0.2</v>
@@ -2098,12 +2775,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="42" spans="2:15">
-      <c r="B42" t="s">
-        <v>15</v>
-      </c>
+    <row r="42" spans="4:15">
       <c r="L42" s="3" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="M42" s="9">
         <v>0.6</v>
@@ -2115,12 +2789,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="43" spans="2:15">
+    <row r="43" spans="4:15">
       <c r="D43" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="F43" t="s">
+        <v>28</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="M43" s="8">
         <v>0.2</v>
@@ -2132,7 +2809,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="44" spans="2:15" ht="30">
+    <row r="44" spans="4:15" ht="30">
       <c r="D44">
         <v>0.2</v>
       </c>
@@ -2143,7 +2820,7 @@
         <v>0.34510000000000002</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="M44" s="9">
         <v>0</v>
@@ -2155,7 +2832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:15">
+    <row r="45" spans="4:15">
       <c r="D45">
         <v>0.2</v>
       </c>
@@ -2166,7 +2843,7 @@
         <v>0.28549999999999998</v>
       </c>
     </row>
-    <row r="46" spans="2:15">
+    <row r="46" spans="4:15">
       <c r="D46">
         <v>0.6</v>
       </c>
@@ -2177,7 +2854,7 @@
         <v>0.17030000000000001</v>
       </c>
     </row>
-    <row r="47" spans="2:15">
+    <row r="47" spans="4:15">
       <c r="D47">
         <v>0</v>
       </c>
@@ -2188,7 +2865,7 @@
         <v>-0.1452</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="4:15">
       <c r="E48">
         <v>1</v>
       </c>
@@ -2207,15 +2884,16 @@
     <row r="50" spans="3:15">
       <c r="M50" s="2"/>
       <c r="N50" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="3:15">
-      <c r="M51" s="3" t="s">
-        <v>6</v>
+      <c r="M51" s="3" t="str">
+        <f>G28</f>
+        <v>s1</v>
       </c>
       <c r="N51" s="8">
         <v>14</v>
@@ -2225,8 +2903,9 @@
       </c>
     </row>
     <row r="52" spans="3:15">
-      <c r="M52" s="3" t="s">
-        <v>7</v>
+      <c r="M52" s="3" t="str">
+        <f t="shared" ref="M52:M56" si="0">G29</f>
+        <v>s2</v>
       </c>
       <c r="N52" s="9">
         <v>15</v>
@@ -2237,17 +2916,18 @@
     </row>
     <row r="53" spans="3:15">
       <c r="C53" s="2"/>
-      <c r="D53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M53" s="3" t="s">
-        <v>8</v>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="str">
+        <f>D35</f>
+        <v>w3</v>
+      </c>
+      <c r="F53" s="3" t="str">
+        <f>D43</f>
+        <v>w4</v>
+      </c>
+      <c r="M53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>s3</v>
       </c>
       <c r="N53" s="8">
         <v>16</v>
@@ -2257,20 +2937,25 @@
       </c>
     </row>
     <row r="54" spans="3:15">
-      <c r="C54" s="3" t="s">
-        <v>19</v>
+      <c r="C54" s="3" t="str">
+        <f>G28</f>
+        <v>s1</v>
       </c>
       <c r="D54" s="4">
+        <f>F28</f>
         <v>-0.2384</v>
       </c>
       <c r="E54" s="5">
+        <f>F36</f>
         <v>0.32669999999999999</v>
       </c>
       <c r="F54" s="5">
+        <f>F44</f>
         <v>0.34510000000000002</v>
       </c>
-      <c r="M54" s="7" t="s">
-        <v>9</v>
+      <c r="M54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>s4</v>
       </c>
       <c r="N54" s="9">
         <v>18</v>
@@ -2280,20 +2965,25 @@
       </c>
     </row>
     <row r="55" spans="3:15">
-      <c r="C55" s="3" t="s">
-        <v>20</v>
+      <c r="C55" s="3" t="str">
+        <f t="shared" ref="C55:C59" si="1">G29</f>
+        <v>s2</v>
       </c>
       <c r="D55" s="6">
+        <f t="shared" ref="D55:D59" si="2">F29</f>
         <v>8.0299999999999996E-2</v>
       </c>
       <c r="E55" s="6">
+        <f t="shared" ref="E55:E59" si="3">F37</f>
         <v>0.29149999999999998</v>
       </c>
       <c r="F55" s="6">
+        <f t="shared" ref="F55:F59" si="4">F45</f>
         <v>0.28549999999999998</v>
       </c>
-      <c r="M55" s="3" t="s">
-        <v>10</v>
+      <c r="M55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>s5</v>
       </c>
       <c r="N55" s="4">
         <v>19</v>
@@ -2303,20 +2993,25 @@
       </c>
     </row>
     <row r="56" spans="3:15">
-      <c r="C56" s="3" t="s">
-        <v>21</v>
+      <c r="C56" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>s3</v>
       </c>
       <c r="D56" s="5">
+        <f t="shared" si="2"/>
         <v>0.12189999999999999</v>
       </c>
       <c r="E56" s="4">
+        <f t="shared" si="3"/>
         <v>0.1731</v>
       </c>
       <c r="F56" s="4">
+        <f t="shared" si="4"/>
         <v>0.17030000000000001</v>
       </c>
-      <c r="M56" s="3" t="s">
-        <v>11</v>
+      <c r="M56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>s6</v>
       </c>
       <c r="N56" s="6">
         <v>20</v>
@@ -2326,73 +3021,197 @@
       </c>
     </row>
     <row r="57" spans="3:15">
-      <c r="C57" s="3" t="s">
-        <v>22</v>
+      <c r="C57" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>s4</v>
       </c>
       <c r="D57" s="6">
+        <f t="shared" si="2"/>
         <v>2.98E-2</v>
       </c>
       <c r="E57" s="6">
+        <f t="shared" si="3"/>
         <v>-0.1288</v>
       </c>
       <c r="F57" s="6">
+        <f t="shared" si="4"/>
         <v>-0.1452</v>
       </c>
     </row>
     <row r="58" spans="3:15">
-      <c r="C58" s="3" t="s">
-        <v>23</v>
+      <c r="C58" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>s5</v>
       </c>
       <c r="D58" s="4">
+        <f t="shared" si="2"/>
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="E58" s="4">
+        <f t="shared" si="3"/>
         <v>-0.26900000000000002</v>
       </c>
       <c r="F58" s="4">
+        <f t="shared" si="4"/>
         <v>-0.28089999999999998</v>
       </c>
     </row>
     <row r="59" spans="3:15">
-      <c r="C59" s="3" t="s">
-        <v>24</v>
+      <c r="C59" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>s6</v>
       </c>
       <c r="D59" s="6">
+        <f t="shared" si="2"/>
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="E59" s="6">
+        <f t="shared" si="3"/>
         <v>-0.39329999999999998</v>
       </c>
       <c r="F59" s="6">
+        <f t="shared" si="4"/>
         <v>-0.37490000000000001</v>
       </c>
-      <c r="L59" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="3:15">
-      <c r="L60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="61" spans="3:15">
-      <c r="L61" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="62" spans="3:15">
-      <c r="L62" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="63" spans="3:15">
-      <c r="L63" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" spans="3:15">
-      <c r="L64" t="s">
-        <v>36</v>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="D67" t="s">
+        <v>2</v>
+      </c>
+      <c r="F67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="14"/>
+      <c r="D68">
+        <v>0.33</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>0.25009999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69" s="15"/>
+      <c r="D69">
+        <v>0.23</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>0.24510000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="14"/>
+      <c r="D70">
+        <v>0.37</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>0.15409999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="16"/>
+      <c r="D71">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>-0.1099</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>-0.22550000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>-0.31390000000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="4:6">
+      <c r="D87" t="s">
+        <v>3</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6">
+      <c r="D88">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>0.18809999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="4:6">
+      <c r="D89">
+        <v>0.27</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89">
+        <v>0.23169999999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6">
+      <c r="D90">
+        <v>0.12</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>0.1527</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6">
+      <c r="D91">
+        <v>0.06</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>-8.5800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="4:6">
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>-0.1948</v>
+      </c>
+    </row>
+    <row r="93" spans="4:6">
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>-0.29189999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2404,12 +3223,1027 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D34" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="7" width="6.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.23</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.37</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30">
+      <c r="A9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="I12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="I13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="N13" s="8">
+        <v>0.83330000000000004</v>
+      </c>
+      <c r="O13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="N14" s="9">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="O14" s="9">
+        <v>0.83330000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="I15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0</v>
+      </c>
+      <c r="K15" s="8">
+        <v>0</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="N15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0.66669999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="I16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0</v>
+      </c>
+      <c r="N16" s="9">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="O16" s="9">
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="9:15">
+      <c r="I17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0</v>
+      </c>
+      <c r="N17" s="8">
+        <v>0</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="9:15">
+      <c r="I18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0</v>
+      </c>
+      <c r="N18" s="9">
+        <v>0</v>
+      </c>
+      <c r="O18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="9:15">
+      <c r="I20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="9:15">
+      <c r="I21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0</v>
+      </c>
+      <c r="L21" s="8">
+        <v>0</v>
+      </c>
+      <c r="M21" s="8">
+        <v>0</v>
+      </c>
+      <c r="N21" s="8">
+        <v>0</v>
+      </c>
+      <c r="O21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="9:15">
+      <c r="I22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0.57069999999999999</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0</v>
+      </c>
+      <c r="M22" s="9">
+        <v>0</v>
+      </c>
+      <c r="N22" s="9">
+        <v>0</v>
+      </c>
+      <c r="O22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="9:15">
+      <c r="I23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="8">
+        <v>0.73740000000000006</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="L23" s="8">
+        <v>0</v>
+      </c>
+      <c r="M23" s="8">
+        <v>0</v>
+      </c>
+      <c r="N23" s="8">
+        <v>0</v>
+      </c>
+      <c r="O23" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="9:15">
+      <c r="I24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0.84109999999999996</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0.27039999999999997</v>
+      </c>
+      <c r="L24" s="9">
+        <v>0.1037</v>
+      </c>
+      <c r="M24" s="9">
+        <v>0</v>
+      </c>
+      <c r="N24" s="9">
+        <v>0</v>
+      </c>
+      <c r="O24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="9:15">
+      <c r="I25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="8">
+        <v>0.91420000000000001</v>
+      </c>
+      <c r="K25" s="8">
+        <v>0.34350000000000003</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0.17680000000000001</v>
+      </c>
+      <c r="M25" s="8">
+        <v>7.3099999999999998E-2</v>
+      </c>
+      <c r="N25" s="8">
+        <v>0</v>
+      </c>
+      <c r="O25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="9:15">
+      <c r="I26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="17">
+        <v>1</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0.42930000000000001</v>
+      </c>
+      <c r="L26" s="9">
+        <v>0.2626</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0.15890000000000001</v>
+      </c>
+      <c r="N26" s="9">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="O26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="9:15">
+      <c r="I28" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="9:15">
+      <c r="I29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0</v>
+      </c>
+      <c r="K29" s="8">
+        <v>0.21740000000000001</v>
+      </c>
+      <c r="L29" s="8">
+        <v>0.3775</v>
+      </c>
+      <c r="M29" s="8">
+        <v>0.73909999999999998</v>
+      </c>
+      <c r="N29" s="8">
+        <v>0.89629999999999999</v>
+      </c>
+      <c r="O29" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="9:15">
+      <c r="I30" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0</v>
+      </c>
+      <c r="K30" s="9">
+        <v>0</v>
+      </c>
+      <c r="L30" s="9">
+        <v>0.16009999999999999</v>
+      </c>
+      <c r="M30" s="9">
+        <v>0.52170000000000005</v>
+      </c>
+      <c r="N30" s="9">
+        <v>0.67889999999999995</v>
+      </c>
+      <c r="O30" s="9">
+        <v>0.78259999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="9:15">
+      <c r="I31" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0</v>
+      </c>
+      <c r="K31" s="8">
+        <v>0</v>
+      </c>
+      <c r="L31" s="8">
+        <v>0</v>
+      </c>
+      <c r="M31" s="8">
+        <v>0.36159999999999998</v>
+      </c>
+      <c r="N31" s="8">
+        <v>0.51890000000000003</v>
+      </c>
+      <c r="O31" s="8">
+        <v>0.62250000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="9:15">
+      <c r="I32" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0</v>
+      </c>
+      <c r="L32" s="9">
+        <v>0</v>
+      </c>
+      <c r="M32" s="9">
+        <v>0</v>
+      </c>
+      <c r="N32" s="9">
+        <v>0.1573</v>
+      </c>
+      <c r="O32" s="9">
+        <v>0.26090000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="9:15">
+      <c r="I33" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="8">
+        <v>0</v>
+      </c>
+      <c r="K33" s="8">
+        <v>0</v>
+      </c>
+      <c r="L33" s="8">
+        <v>0</v>
+      </c>
+      <c r="M33" s="8">
+        <v>0</v>
+      </c>
+      <c r="N33" s="8">
+        <v>0</v>
+      </c>
+      <c r="O33" s="8">
+        <v>0.1037</v>
+      </c>
+    </row>
+    <row r="34" spans="9:15">
+      <c r="I34" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="17">
+        <v>0</v>
+      </c>
+      <c r="K34" s="9">
+        <v>0</v>
+      </c>
+      <c r="L34" s="9">
+        <v>0</v>
+      </c>
+      <c r="M34" s="9">
+        <v>0</v>
+      </c>
+      <c r="N34" s="9">
+        <v>0</v>
+      </c>
+      <c r="O34" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:15" ht="30">
+      <c r="I36" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="9:15">
+      <c r="I37" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="8">
+        <v>0</v>
+      </c>
+      <c r="K37" s="8">
+        <v>1</v>
+      </c>
+      <c r="L37" s="8">
+        <v>1</v>
+      </c>
+      <c r="M37" s="8">
+        <v>1</v>
+      </c>
+      <c r="N37" s="8">
+        <v>1</v>
+      </c>
+      <c r="O37" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="9:15">
+      <c r="I38" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="9">
+        <v>1</v>
+      </c>
+      <c r="K38" s="9">
+        <v>0</v>
+      </c>
+      <c r="L38" s="9">
+        <v>1</v>
+      </c>
+      <c r="M38" s="9">
+        <v>1</v>
+      </c>
+      <c r="N38" s="9">
+        <v>1</v>
+      </c>
+      <c r="O38" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="9:15">
+      <c r="I39" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="8">
+        <v>1</v>
+      </c>
+      <c r="K39" s="8">
+        <v>1</v>
+      </c>
+      <c r="L39" s="8">
+        <v>0</v>
+      </c>
+      <c r="M39" s="8">
+        <v>1</v>
+      </c>
+      <c r="N39" s="8">
+        <v>1</v>
+      </c>
+      <c r="O39" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="9:15">
+      <c r="I40" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="9">
+        <v>1</v>
+      </c>
+      <c r="K40" s="9">
+        <v>1</v>
+      </c>
+      <c r="L40" s="9">
+        <v>1</v>
+      </c>
+      <c r="M40" s="9">
+        <v>0</v>
+      </c>
+      <c r="N40" s="9">
+        <v>1</v>
+      </c>
+      <c r="O40" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="9:15">
+      <c r="I41" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" s="8">
+        <v>1</v>
+      </c>
+      <c r="K41" s="8">
+        <v>1</v>
+      </c>
+      <c r="L41" s="8">
+        <v>1</v>
+      </c>
+      <c r="M41" s="8">
+        <v>1</v>
+      </c>
+      <c r="N41" s="8">
+        <v>0</v>
+      </c>
+      <c r="O41" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="9:15">
+      <c r="I42" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="17">
+        <v>1</v>
+      </c>
+      <c r="K42" s="9">
+        <v>1</v>
+      </c>
+      <c r="L42" s="9">
+        <v>1</v>
+      </c>
+      <c r="M42" s="9">
+        <v>1</v>
+      </c>
+      <c r="N42" s="9">
+        <v>1</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="9:15">
+      <c r="I44" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O44" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="9:15">
+      <c r="I45" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J45" s="8">
+        <v>0</v>
+      </c>
+      <c r="K45" s="8">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="L45" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="M45" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N45" s="8">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="O45" s="19">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="46" spans="9:15">
+      <c r="I46" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J46" s="9">
+        <v>0.81269999999999998</v>
+      </c>
+      <c r="K46" s="9">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="L46" s="9">
+        <v>0.1086</v>
+      </c>
+      <c r="M46" s="9">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="N46" s="9">
+        <v>1.72E-2</v>
+      </c>
+      <c r="O46" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="9:15">
+      <c r="I47" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J47" s="8">
+        <v>0</v>
+      </c>
+      <c r="K47" s="8">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="L47" s="8">
+        <v>0.1075</v>
+      </c>
+      <c r="M47" s="8">
+        <v>0.32450000000000001</v>
+      </c>
+      <c r="N47" s="8">
+        <v>0.45029999999999998</v>
+      </c>
+      <c r="O47" s="8">
+        <v>0.55389999999999995</v>
+      </c>
+    </row>
+    <row r="48" spans="9:15" ht="30">
+      <c r="I48" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J48" s="9">
+        <v>1</v>
+      </c>
+      <c r="K48" s="9">
+        <v>1</v>
+      </c>
+      <c r="L48" s="9">
+        <v>1</v>
+      </c>
+      <c r="M48" s="9">
+        <v>1</v>
+      </c>
+      <c r="N48" s="9">
+        <v>1</v>
+      </c>
+      <c r="O48" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="17:21" ht="30">
+      <c r="Q50" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="R50" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="S50" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="T50" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="U50" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="17:21">
+      <c r="Q51" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="R51" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="S51" s="8">
+        <v>0</v>
+      </c>
+      <c r="T51" s="8">
+        <v>0.64610000000000001</v>
+      </c>
+      <c r="U51" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="17:21">
+      <c r="Q52" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="R52" s="9">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="S52" s="9">
+        <v>0.11409999999999999</v>
+      </c>
+      <c r="T52" s="9">
+        <v>0.42870000000000003</v>
+      </c>
+      <c r="U52" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="17:21">
+      <c r="Q53" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="R53" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="S53" s="8">
+        <v>0.18079999999999999</v>
+      </c>
+      <c r="T53" s="8">
+        <v>0.30059999999999998</v>
+      </c>
+      <c r="U53" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="17:21">
+      <c r="Q54" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="R54" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="S54" s="9">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="T54" s="9">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="U54" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="17:21">
+      <c r="Q55" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="R55" s="8">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="S55" s="8">
+        <v>0.30149999999999999</v>
+      </c>
+      <c r="T55" s="8">
+        <v>2.07E-2</v>
+      </c>
+      <c r="U55" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="17:21">
+      <c r="Q56" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="R56" s="17">
+        <v>0</v>
+      </c>
+      <c r="S56" s="9">
+        <v>0.38729999999999998</v>
+      </c>
+      <c r="T56" s="9">
+        <v>0</v>
+      </c>
+      <c r="U56" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>